<commit_message>
configuración dns - dominio mileto.com.co
</commit_message>
<xml_diff>
--- a/static/models/templatePredictorsDemand.xlsx
+++ b/static/models/templatePredictorsDemand.xlsx
@@ -438,7 +438,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>21:40</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -446,7 +446,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>19:22</t>
+          <t>20:40</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -454,7 +454,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>18:22</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
@@ -462,7 +462,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>17:22</t>
+          <t>18:40</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
@@ -470,7 +470,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>16:22</t>
+          <t>17:40</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
@@ -478,7 +478,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>15:22</t>
+          <t>16:40</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
@@ -486,7 +486,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>14:22</t>
+          <t>15:40</t>
         </is>
       </c>
       <c r="B8" t="inlineStr"/>
@@ -494,7 +494,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>13:22</t>
+          <t>14:40</t>
         </is>
       </c>
       <c r="B9" t="inlineStr"/>
@@ -502,7 +502,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>12:22</t>
+          <t>13:40</t>
         </is>
       </c>
       <c r="B10" t="inlineStr"/>
@@ -510,7 +510,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>11:22</t>
+          <t>12:40</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
@@ -518,7 +518,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>10:22</t>
+          <t>11:40</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
@@ -526,7 +526,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>09:22</t>
+          <t>10:40</t>
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
@@ -534,7 +534,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>08:22</t>
+          <t>09:40</t>
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
@@ -542,7 +542,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>07:22</t>
+          <t>08:40</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
@@ -550,7 +550,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>06:22</t>
+          <t>07:40</t>
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
@@ -558,7 +558,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>05:22</t>
+          <t>06:40</t>
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
@@ -566,7 +566,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>04:22</t>
+          <t>05:40</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
@@ -574,7 +574,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>03:22</t>
+          <t>04:40</t>
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
@@ -582,7 +582,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>02:22</t>
+          <t>03:40</t>
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
@@ -590,7 +590,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>01:22</t>
+          <t>02:40</t>
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
@@ -598,7 +598,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>00:22</t>
+          <t>01:40</t>
         </is>
       </c>
       <c r="B22" t="inlineStr"/>
@@ -606,7 +606,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>23:22</t>
+          <t>00:40</t>
         </is>
       </c>
       <c r="B23" t="inlineStr"/>
@@ -614,7 +614,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>22:22</t>
+          <t>23:40</t>
         </is>
       </c>
       <c r="B24" t="inlineStr"/>
@@ -622,7 +622,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>21:22</t>
+          <t>22:40</t>
         </is>
       </c>
       <c r="B25" t="inlineStr"/>
@@ -661,7 +661,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2023-03-23 21:22</t>
+          <t>2023-05-02 22:40</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -700,7 +700,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2023-03-17 21:22</t>
+          <t>2023-04-26 22:40</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -708,7 +708,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2023-03-17 20:22</t>
+          <t>2023-04-26 21:40</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -716,7 +716,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2023-03-17 19:22</t>
+          <t>2023-04-26 20:40</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
@@ -724,7 +724,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2023-03-17 18:22</t>
+          <t>2023-04-26 19:40</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
@@ -732,7 +732,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2023-03-17 17:22</t>
+          <t>2023-04-26 18:40</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
@@ -740,7 +740,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2023-03-17 16:22</t>
+          <t>2023-04-26 17:40</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
@@ -748,7 +748,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2023-03-17 15:22</t>
+          <t>2023-04-26 16:40</t>
         </is>
       </c>
       <c r="B8" t="inlineStr"/>
@@ -756,7 +756,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2023-03-17 14:22</t>
+          <t>2023-04-26 15:40</t>
         </is>
       </c>
       <c r="B9" t="inlineStr"/>
@@ -764,7 +764,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2023-03-17 13:22</t>
+          <t>2023-04-26 14:40</t>
         </is>
       </c>
       <c r="B10" t="inlineStr"/>
@@ -772,7 +772,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2023-03-17 12:22</t>
+          <t>2023-04-26 13:40</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
@@ -780,7 +780,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2023-03-17 11:22</t>
+          <t>2023-04-26 12:40</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
@@ -788,7 +788,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2023-03-17 10:22</t>
+          <t>2023-04-26 11:40</t>
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
@@ -796,7 +796,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2023-03-17 09:22</t>
+          <t>2023-04-26 10:40</t>
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
@@ -804,7 +804,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2023-03-17 08:22</t>
+          <t>2023-04-26 09:40</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
@@ -812,7 +812,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2023-03-17 07:22</t>
+          <t>2023-04-26 08:40</t>
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
@@ -820,7 +820,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2023-03-17 06:22</t>
+          <t>2023-04-26 07:40</t>
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
@@ -828,7 +828,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2023-03-17 05:22</t>
+          <t>2023-04-26 06:40</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
@@ -836,7 +836,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2023-03-17 04:22</t>
+          <t>2023-04-26 05:40</t>
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
@@ -844,7 +844,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2023-03-17 03:22</t>
+          <t>2023-04-26 04:40</t>
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
@@ -852,7 +852,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2023-03-17 02:22</t>
+          <t>2023-04-26 03:40</t>
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
@@ -860,7 +860,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2023-03-17 01:22</t>
+          <t>2023-04-26 02:40</t>
         </is>
       </c>
       <c r="B22" t="inlineStr"/>
@@ -868,7 +868,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2023-03-17 00:22</t>
+          <t>2023-04-26 01:40</t>
         </is>
       </c>
       <c r="B23" t="inlineStr"/>
@@ -876,7 +876,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2023-03-16 23:22</t>
+          <t>2023-04-26 00:40</t>
         </is>
       </c>
       <c r="B24" t="inlineStr"/>
@@ -884,7 +884,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2023-03-16 22:22</t>
+          <t>2023-04-25 23:40</t>
         </is>
       </c>
       <c r="B25" t="inlineStr"/>

</xml_diff>

<commit_message>
cambios en evaluate y testing
</commit_message>
<xml_diff>
--- a/static/models/templatePredictorsDemand.xlsx
+++ b/static/models/templatePredictorsDemand.xlsx
@@ -438,7 +438,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>21:40</t>
+          <t>2023-05-06 14:03</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -446,7 +446,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>20:40</t>
+          <t>2023-05-06 13:03</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -454,7 +454,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>2023-05-06 12:03</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
@@ -462,7 +462,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>18:40</t>
+          <t>2023-05-06 11:03</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
@@ -470,7 +470,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>17:40</t>
+          <t>2023-05-06 10:03</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
@@ -478,7 +478,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>16:40</t>
+          <t>2023-05-06 09:03</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
@@ -486,7 +486,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>15:40</t>
+          <t>2023-05-06 08:03</t>
         </is>
       </c>
       <c r="B8" t="inlineStr"/>
@@ -494,7 +494,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>14:40</t>
+          <t>2023-05-06 07:03</t>
         </is>
       </c>
       <c r="B9" t="inlineStr"/>
@@ -502,7 +502,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>13:40</t>
+          <t>2023-05-06 06:03</t>
         </is>
       </c>
       <c r="B10" t="inlineStr"/>
@@ -510,7 +510,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>12:40</t>
+          <t>2023-05-06 05:03</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
@@ -518,7 +518,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>11:40</t>
+          <t>2023-05-06 04:03</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
@@ -526,7 +526,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>10:40</t>
+          <t>2023-05-06 03:03</t>
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
@@ -534,7 +534,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>09:40</t>
+          <t>2023-05-06 02:03</t>
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
@@ -542,7 +542,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>08:40</t>
+          <t>2023-05-06 01:03</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
@@ -550,7 +550,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>07:40</t>
+          <t>2023-05-06 00:03</t>
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
@@ -558,7 +558,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>06:40</t>
+          <t>2023-05-05 23:03</t>
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
@@ -566,7 +566,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>05:40</t>
+          <t>2023-05-05 22:03</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
@@ -574,7 +574,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>04:40</t>
+          <t>2023-05-05 21:03</t>
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
@@ -582,7 +582,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>03:40</t>
+          <t>2023-05-05 20:03</t>
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
@@ -590,7 +590,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>02:40</t>
+          <t>2023-05-05 19:03</t>
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
@@ -598,7 +598,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>01:40</t>
+          <t>2023-05-05 18:03</t>
         </is>
       </c>
       <c r="B22" t="inlineStr"/>
@@ -606,7 +606,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>00:40</t>
+          <t>2023-05-05 17:03</t>
         </is>
       </c>
       <c r="B23" t="inlineStr"/>
@@ -614,7 +614,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>23:40</t>
+          <t>2023-05-05 16:03</t>
         </is>
       </c>
       <c r="B24" t="inlineStr"/>
@@ -622,7 +622,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>22:40</t>
+          <t>2023-05-05 15:03</t>
         </is>
       </c>
       <c r="B25" t="inlineStr"/>
@@ -638,7 +638,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -661,10 +661,194 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2023-05-02 22:40</t>
+          <t>2023-05-05 15:03</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2023-05-05 14:03</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2023-05-05 13:03</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2023-05-05 12:03</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2023-05-05 11:03</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2023-05-05 10:03</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2023-05-05 09:03</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2023-05-05 08:03</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2023-05-05 07:03</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2023-05-05 06:03</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2023-05-05 05:03</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2023-05-05 04:03</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2023-05-05 03:03</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2023-05-05 02:03</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2023-05-05 01:03</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2023-05-05 00:03</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2023-05-04 23:03</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2023-05-04 22:03</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2023-05-04 21:03</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2023-05-04 20:03</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2023-05-04 19:03</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2023-05-04 18:03</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2023-05-04 17:03</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2023-05-04 16:03</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -700,7 +884,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2023-04-26 22:40</t>
+          <t>2023-04-29 15:03</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -708,7 +892,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2023-04-26 21:40</t>
+          <t>2023-04-29 14:03</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -716,7 +900,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2023-04-26 20:40</t>
+          <t>2023-04-29 13:03</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
@@ -724,7 +908,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2023-04-26 19:40</t>
+          <t>2023-04-29 12:03</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
@@ -732,7 +916,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2023-04-26 18:40</t>
+          <t>2023-04-29 11:03</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
@@ -740,7 +924,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2023-04-26 17:40</t>
+          <t>2023-04-29 10:03</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
@@ -748,7 +932,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2023-04-26 16:40</t>
+          <t>2023-04-29 09:03</t>
         </is>
       </c>
       <c r="B8" t="inlineStr"/>
@@ -756,7 +940,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2023-04-26 15:40</t>
+          <t>2023-04-29 08:03</t>
         </is>
       </c>
       <c r="B9" t="inlineStr"/>
@@ -764,7 +948,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2023-04-26 14:40</t>
+          <t>2023-04-29 07:03</t>
         </is>
       </c>
       <c r="B10" t="inlineStr"/>
@@ -772,7 +956,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2023-04-26 13:40</t>
+          <t>2023-04-29 06:03</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
@@ -780,7 +964,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2023-04-26 12:40</t>
+          <t>2023-04-29 05:03</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
@@ -788,7 +972,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2023-04-26 11:40</t>
+          <t>2023-04-29 04:03</t>
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
@@ -796,7 +980,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2023-04-26 10:40</t>
+          <t>2023-04-29 03:03</t>
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
@@ -804,7 +988,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2023-04-26 09:40</t>
+          <t>2023-04-29 02:03</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
@@ -812,7 +996,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2023-04-26 08:40</t>
+          <t>2023-04-29 01:03</t>
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
@@ -820,7 +1004,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2023-04-26 07:40</t>
+          <t>2023-04-29 00:03</t>
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
@@ -828,7 +1012,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2023-04-26 06:40</t>
+          <t>2023-04-28 23:03</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
@@ -836,7 +1020,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2023-04-26 05:40</t>
+          <t>2023-04-28 22:03</t>
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
@@ -844,7 +1028,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2023-04-26 04:40</t>
+          <t>2023-04-28 21:03</t>
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
@@ -852,7 +1036,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2023-04-26 03:40</t>
+          <t>2023-04-28 20:03</t>
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
@@ -860,7 +1044,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2023-04-26 02:40</t>
+          <t>2023-04-28 19:03</t>
         </is>
       </c>
       <c r="B22" t="inlineStr"/>
@@ -868,7 +1052,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2023-04-26 01:40</t>
+          <t>2023-04-28 18:03</t>
         </is>
       </c>
       <c r="B23" t="inlineStr"/>
@@ -876,7 +1060,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2023-04-26 00:40</t>
+          <t>2023-04-28 17:03</t>
         </is>
       </c>
       <c r="B24" t="inlineStr"/>
@@ -884,7 +1068,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2023-04-25 23:40</t>
+          <t>2023-04-28 16:03</t>
         </is>
       </c>
       <c r="B25" t="inlineStr"/>

</xml_diff>

<commit_message>
gamma y C variables
</commit_message>
<xml_diff>
--- a/static/models/templatePredictorsDemand.xlsx
+++ b/static/models/templatePredictorsDemand.xlsx
@@ -438,7 +438,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2023-05-06 14:03</t>
+          <t>2023-05-12 07:30</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -446,7 +446,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2023-05-06 13:03</t>
+          <t>2023-05-12 06:30</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -454,7 +454,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2023-05-06 12:03</t>
+          <t>2023-05-12 05:30</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
@@ -462,7 +462,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2023-05-06 11:03</t>
+          <t>2023-05-12 04:30</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
@@ -470,7 +470,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2023-05-06 10:03</t>
+          <t>2023-05-12 03:30</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
@@ -478,7 +478,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2023-05-06 09:03</t>
+          <t>2023-05-12 02:30</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
@@ -486,7 +486,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2023-05-06 08:03</t>
+          <t>2023-05-12 01:30</t>
         </is>
       </c>
       <c r="B8" t="inlineStr"/>
@@ -494,7 +494,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2023-05-06 07:03</t>
+          <t>2023-05-12 00:30</t>
         </is>
       </c>
       <c r="B9" t="inlineStr"/>
@@ -502,7 +502,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2023-05-06 06:03</t>
+          <t>2023-05-11 23:30</t>
         </is>
       </c>
       <c r="B10" t="inlineStr"/>
@@ -510,7 +510,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2023-05-06 05:03</t>
+          <t>2023-05-11 22:30</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
@@ -518,7 +518,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2023-05-06 04:03</t>
+          <t>2023-05-11 21:30</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
@@ -526,7 +526,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2023-05-06 03:03</t>
+          <t>2023-05-11 20:30</t>
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
@@ -534,7 +534,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2023-05-06 02:03</t>
+          <t>2023-05-11 19:30</t>
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
@@ -542,7 +542,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2023-05-06 01:03</t>
+          <t>2023-05-11 18:30</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
@@ -550,7 +550,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2023-05-06 00:03</t>
+          <t>2023-05-11 17:30</t>
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
@@ -558,7 +558,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2023-05-05 23:03</t>
+          <t>2023-05-11 16:30</t>
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
@@ -566,7 +566,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2023-05-05 22:03</t>
+          <t>2023-05-11 15:30</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
@@ -574,7 +574,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2023-05-05 21:03</t>
+          <t>2023-05-11 14:30</t>
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
@@ -582,7 +582,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2023-05-05 20:03</t>
+          <t>2023-05-11 13:30</t>
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
@@ -590,7 +590,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2023-05-05 19:03</t>
+          <t>2023-05-11 12:30</t>
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
@@ -598,7 +598,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2023-05-05 18:03</t>
+          <t>2023-05-11 11:30</t>
         </is>
       </c>
       <c r="B22" t="inlineStr"/>
@@ -606,7 +606,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2023-05-05 17:03</t>
+          <t>2023-05-11 10:30</t>
         </is>
       </c>
       <c r="B23" t="inlineStr"/>
@@ -614,7 +614,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2023-05-05 16:03</t>
+          <t>2023-05-11 09:30</t>
         </is>
       </c>
       <c r="B24" t="inlineStr"/>
@@ -622,7 +622,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2023-05-05 15:03</t>
+          <t>2023-05-11 08:30</t>
         </is>
       </c>
       <c r="B25" t="inlineStr"/>
@@ -661,7 +661,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2023-05-05 15:03</t>
+          <t>2023-05-11 08:30</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -669,7 +669,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2023-05-05 14:03</t>
+          <t>2023-05-11 07:30</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -677,7 +677,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2023-05-05 13:03</t>
+          <t>2023-05-11 06:30</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
@@ -685,7 +685,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2023-05-05 12:03</t>
+          <t>2023-05-11 05:30</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
@@ -693,7 +693,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2023-05-05 11:03</t>
+          <t>2023-05-11 04:30</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
@@ -701,7 +701,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2023-05-05 10:03</t>
+          <t>2023-05-11 03:30</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
@@ -709,7 +709,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2023-05-05 09:03</t>
+          <t>2023-05-11 02:30</t>
         </is>
       </c>
       <c r="B8" t="inlineStr"/>
@@ -717,7 +717,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2023-05-05 08:03</t>
+          <t>2023-05-11 01:30</t>
         </is>
       </c>
       <c r="B9" t="inlineStr"/>
@@ -725,7 +725,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2023-05-05 07:03</t>
+          <t>2023-05-11 00:30</t>
         </is>
       </c>
       <c r="B10" t="inlineStr"/>
@@ -733,7 +733,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2023-05-05 06:03</t>
+          <t>2023-05-10 23:30</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
@@ -741,7 +741,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2023-05-05 05:03</t>
+          <t>2023-05-10 22:30</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
@@ -749,7 +749,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2023-05-05 04:03</t>
+          <t>2023-05-10 21:30</t>
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
@@ -757,7 +757,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2023-05-05 03:03</t>
+          <t>2023-05-10 20:30</t>
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
@@ -765,7 +765,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2023-05-05 02:03</t>
+          <t>2023-05-10 19:30</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
@@ -773,7 +773,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2023-05-05 01:03</t>
+          <t>2023-05-10 18:30</t>
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
@@ -781,7 +781,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2023-05-05 00:03</t>
+          <t>2023-05-10 17:30</t>
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
@@ -789,7 +789,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2023-05-04 23:03</t>
+          <t>2023-05-10 16:30</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
@@ -797,7 +797,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2023-05-04 22:03</t>
+          <t>2023-05-10 15:30</t>
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
@@ -805,7 +805,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2023-05-04 21:03</t>
+          <t>2023-05-10 14:30</t>
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
@@ -813,7 +813,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2023-05-04 20:03</t>
+          <t>2023-05-10 13:30</t>
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
@@ -821,7 +821,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2023-05-04 19:03</t>
+          <t>2023-05-10 12:30</t>
         </is>
       </c>
       <c r="B22" t="inlineStr"/>
@@ -829,7 +829,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2023-05-04 18:03</t>
+          <t>2023-05-10 11:30</t>
         </is>
       </c>
       <c r="B23" t="inlineStr"/>
@@ -837,7 +837,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2023-05-04 17:03</t>
+          <t>2023-05-10 10:30</t>
         </is>
       </c>
       <c r="B24" t="inlineStr"/>
@@ -845,7 +845,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2023-05-04 16:03</t>
+          <t>2023-05-10 09:30</t>
         </is>
       </c>
       <c r="B25" t="inlineStr"/>
@@ -884,7 +884,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2023-04-29 15:03</t>
+          <t>2023-05-05 08:30</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -892,7 +892,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2023-04-29 14:03</t>
+          <t>2023-05-05 07:30</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -900,7 +900,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2023-04-29 13:03</t>
+          <t>2023-05-05 06:30</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
@@ -908,7 +908,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2023-04-29 12:03</t>
+          <t>2023-05-05 05:30</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
@@ -916,7 +916,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2023-04-29 11:03</t>
+          <t>2023-05-05 04:30</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
@@ -924,7 +924,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2023-04-29 10:03</t>
+          <t>2023-05-05 03:30</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
@@ -932,7 +932,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2023-04-29 09:03</t>
+          <t>2023-05-05 02:30</t>
         </is>
       </c>
       <c r="B8" t="inlineStr"/>
@@ -940,7 +940,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2023-04-29 08:03</t>
+          <t>2023-05-05 01:30</t>
         </is>
       </c>
       <c r="B9" t="inlineStr"/>
@@ -948,7 +948,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2023-04-29 07:03</t>
+          <t>2023-05-05 00:30</t>
         </is>
       </c>
       <c r="B10" t="inlineStr"/>
@@ -956,7 +956,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2023-04-29 06:03</t>
+          <t>2023-05-04 23:30</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
@@ -964,7 +964,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2023-04-29 05:03</t>
+          <t>2023-05-04 22:30</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
@@ -972,7 +972,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2023-04-29 04:03</t>
+          <t>2023-05-04 21:30</t>
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
@@ -980,7 +980,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2023-04-29 03:03</t>
+          <t>2023-05-04 20:30</t>
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
@@ -988,7 +988,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2023-04-29 02:03</t>
+          <t>2023-05-04 19:30</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
@@ -996,7 +996,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2023-04-29 01:03</t>
+          <t>2023-05-04 18:30</t>
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
@@ -1004,7 +1004,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2023-04-29 00:03</t>
+          <t>2023-05-04 17:30</t>
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
@@ -1012,7 +1012,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2023-04-28 23:03</t>
+          <t>2023-05-04 16:30</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
@@ -1020,7 +1020,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2023-04-28 22:03</t>
+          <t>2023-05-04 15:30</t>
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
@@ -1028,7 +1028,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2023-04-28 21:03</t>
+          <t>2023-05-04 14:30</t>
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
@@ -1036,7 +1036,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2023-04-28 20:03</t>
+          <t>2023-05-04 13:30</t>
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
@@ -1044,7 +1044,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2023-04-28 19:03</t>
+          <t>2023-05-04 12:30</t>
         </is>
       </c>
       <c r="B22" t="inlineStr"/>
@@ -1052,7 +1052,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2023-04-28 18:03</t>
+          <t>2023-05-04 11:30</t>
         </is>
       </c>
       <c r="B23" t="inlineStr"/>
@@ -1060,7 +1060,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2023-04-28 17:03</t>
+          <t>2023-05-04 10:30</t>
         </is>
       </c>
       <c r="B24" t="inlineStr"/>
@@ -1068,7 +1068,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2023-04-28 16:03</t>
+          <t>2023-05-04 09:30</t>
         </is>
       </c>
       <c r="B25" t="inlineStr"/>

</xml_diff>